<commit_message>
Docs deleted en replaced
</commit_message>
<xml_diff>
--- a/docs/Projectskills/werk begroting.xlsx
+++ b/docs/Projectskills/werk begroting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\callu\Team Efficient FYS-Project\docs\Projectskills\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\callu\Downloads\Projectplan Team Efficient\Projectskills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCDFB98-32B3-4E88-BEEA-07FFF58F35D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D06FDE0-5F4D-48F6-B520-8FF9F026130D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BE75E16D-561B-4F7C-B366-3E6D0BC44B9A}"/>
   </bookViews>
@@ -482,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3827D50F-C076-472E-AD24-D8FEEAC148E0}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +495,7 @@
     <col min="7" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,11 +526,12 @@
       <c r="J1" s="4">
         <v>44086</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="T1" s="8"/>
+      <c r="W1" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -540,12 +541,13 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="O2" s="7">
+      <c r="T2" s="7"/>
+      <c r="W2" s="7">
         <f>SUM(B2:N2)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -570,12 +572,13 @@
       <c r="J3" s="5">
         <v>1</v>
       </c>
-      <c r="O3" s="8">
+      <c r="T3" s="8"/>
+      <c r="W3" s="8">
         <f>SUM(B3:N3)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -594,12 +597,13 @@
       <c r="I4">
         <v>2</v>
       </c>
-      <c r="O4" s="7">
+      <c r="T4" s="7"/>
+      <c r="W4" s="7">
         <f>SUM(B4:N4)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -624,12 +628,13 @@
       <c r="I5">
         <v>2</v>
       </c>
-      <c r="O5" s="7">
+      <c r="T5" s="7"/>
+      <c r="W5" s="7">
         <f>SUM(B5:N5)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -654,12 +659,13 @@
       <c r="J6">
         <v>1</v>
       </c>
-      <c r="O6" s="7">
+      <c r="T6" s="7"/>
+      <c r="W6" s="7">
         <f>SUM(B6:N6)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -669,12 +675,13 @@
       <c r="H7">
         <v>0.5</v>
       </c>
-      <c r="O7" s="7">
+      <c r="T7" s="7"/>
+      <c r="W7" s="7">
         <f>SUM(A7:N7)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -684,12 +691,13 @@
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="O8" s="7">
+      <c r="T8" s="7"/>
+      <c r="W8" s="7">
         <f>SUM(B8:N8)</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -732,8 +740,9 @@
         <f>SUM(K2:K8)</f>
         <v>0</v>
       </c>
-      <c r="O9" s="7">
-        <f>SUM(O2:O8)</f>
+      <c r="T9" s="7"/>
+      <c r="W9" s="7">
+        <f>SUM(W2:W8)</f>
         <v>64.5</v>
       </c>
     </row>

</xml_diff>